<commit_message>
version 1.0 : Minor Updates in codes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSPACE\SELENIUM_JAVA\RestAssuredFramework_TMB_May23\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B59B40E-F196-45B2-9CE8-FC9CFEA3EDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EFF172-8437-4EE2-8A18-D005871FB589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="runManager" sheetId="2" r:id="rId1"/>
@@ -614,9 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669B42E9-DA3D-4EF6-ACF1-72654820E66A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -637,7 +635,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -645,7 +643,7 @@
         <v>53</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -669,7 +667,7 @@
         <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -677,7 +675,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -690,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
version 1.0 : Minor Bug fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSPACE\SELENIUM_JAVA\RestAssuredFramework_TMB_May23\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EFF172-8437-4EE2-8A18-D005871FB589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4475F6-9F79-42A2-9F24-F9D83962EC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="runManager" sheetId="2" r:id="rId1"/>
-    <sheet name="iterationdata" sheetId="1" r:id="rId2"/>
+    <sheet name="iterationData" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -614,7 +614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669B42E9-DA3D-4EF6-ACF1-72654820E66A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -688,9 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -810,7 +810,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -951,7 +951,7 @@
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
version 1.1 : Refactored code to log response in extent
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSPACE\SELENIUM_JAVA\RestAssuredFramework_TMB_May23\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4475F6-9F79-42A2-9F24-F9D83962EC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1D3214-19D1-42B7-9FE5-A6A1D7FFB946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -614,9 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669B42E9-DA3D-4EF6-ACF1-72654820E66A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>